<commit_message>
set write log to file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan2k\Desktop\job\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C98AA9B-11D9-44D4-8422-1D6CB421D684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B572FB2-33E0-44FD-A411-2C563B45A25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1D58823-75EE-4683-B8B8-D7CEE68BBD40}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L101166" sqref="L101166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>